<commit_message>
Add option to switch between SAFE and WIFM 4.1 at runtime
Update the convergence analysis and more
</commit_message>
<xml_diff>
--- a/SafeCalculations.xlsx
+++ b/SafeCalculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UCDAVIS\IWFM-SAFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F0F6E19-908C-4019-B02D-F73C368DC927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4506D5BC-1799-4CA1-896B-2A324F1E87CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="1050" windowWidth="17805" windowHeight="13770" xr2:uid="{3E1B28E5-C197-4FCE-9C2D-D1E6C61BB483}"/>
+    <workbookView xWindow="-19845" yWindow="285" windowWidth="19965" windowHeight="12765" xr2:uid="{3E1B28E5-C197-4FCE-9C2D-D1E6C61BB483}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>Area</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Qsint</t>
+  </si>
+  <si>
+    <t>rHeadDiff</t>
+  </si>
+  <si>
+    <t>COEFF</t>
   </si>
 </sst>
 </file>
@@ -506,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F48329-6E34-4847-A84B-D178A737002D}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,14 +799,14 @@
       </c>
       <c r="E19">
         <f>B22-B24</f>
-        <v>3.9870122585491998</v>
+        <v>3.3910320009079555</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="3">
         <f>E24*(1+H17*E21+H18*(E21^2))</f>
-        <v>0.34114552081240479</v>
+        <v>0.33565210806616697</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -815,14 +821,14 @@
       </c>
       <c r="E20">
         <f>B23-B21</f>
-        <v>47.618111760979104</v>
+        <v>47.024502896184202</v>
       </c>
       <c r="G20" t="s">
         <v>22</v>
       </c>
       <c r="H20">
         <f>B25-2*(B22-B24)</f>
-        <v>5.3394950845334002</v>
+        <v>5.5421074918243889</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -837,14 +843,14 @@
       </c>
       <c r="E21">
         <f>E19/E20</f>
-        <v>8.3728902955290563E-2</v>
+        <v>7.2112022287493874E-2</v>
       </c>
       <c r="G21" t="s">
         <v>23</v>
       </c>
       <c r="H21">
         <f>H20/2</f>
-        <v>2.6697475422667001</v>
+        <v>2.7710537459121944</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -852,21 +858,21 @@
         <v>9</v>
       </c>
       <c r="B22">
-        <v>97.617012258549195</v>
+        <v>97.021032000907951</v>
       </c>
       <c r="D22" t="s">
         <v>15</v>
       </c>
       <c r="E22">
         <f>B25/E20</f>
-        <v>0.27958940641030688</v>
+        <v>0.26207978255183945</v>
       </c>
       <c r="G22" t="s">
         <v>24</v>
       </c>
       <c r="H22">
         <f>E18/4 - H21 - 2*E20</f>
-        <v>-58.843471064224907</v>
+        <v>-57.757559538280603</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -874,21 +880,21 @@
         <v>10</v>
       </c>
       <c r="B23">
-        <v>97.618111760979104</v>
+        <v>97.024502896184202</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
       </c>
       <c r="E23">
         <f>EXP(-PI()*E22)</f>
-        <v>0.41546536515024318</v>
+        <v>0.4389595903241556</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H23" s="3">
         <f>H19/(1+H19*(H22/E20))</f>
-        <v>0.58977453037676064</v>
+        <v>0.57109202498655431</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -903,14 +909,14 @@
       </c>
       <c r="E24" s="2">
         <f>1/(2*(1 + (1/PI())*LN(2/( 1-SQRT(E23) )  )   ))</f>
-        <v>0.32260138119549098</v>
+        <v>0.31919949653584606</v>
       </c>
       <c r="G24" t="s">
         <v>28</v>
       </c>
       <c r="H24">
         <f>H23/(1+H23*(B26/B19) * B20/(H21+E19))</f>
-        <v>0.2776442267639897</v>
+        <v>0.26245194783303399</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -918,14 +924,14 @@
         <v>14</v>
       </c>
       <c r="B25">
-        <v>13.3135196016318</v>
+        <v>12.3241714936403</v>
       </c>
       <c r="G25" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H25">
         <f>2*B18*B26*H24*30</f>
-        <v>66056.275026151532</v>
+        <v>62441.773953920419</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -935,6 +941,13 @@
       <c r="B26">
         <v>25.377810846560799</v>
       </c>
+      <c r="G26" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26">
+        <f>B22-B23</f>
+        <v>-3.47089527625144E-3</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -942,6 +955,13 @@
       </c>
       <c r="B27">
         <v>25.191798941798901</v>
+      </c>
+      <c r="G27" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27">
+        <f>H26*H25</f>
+        <v>-216.72885825742259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>